<commit_message>
bpnn 0.9672885440459177 0.022652563278844674 0.9704338189815275 0.02219182
</commit_message>
<xml_diff>
--- a/nirs_water_prediction/result/tmp_plsr.xlsx
+++ b/nirs_water_prediction/result/tmp_plsr.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R186"/>
+  <dimension ref="A1:R189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27393,6 +27393,573 @@
         </is>
       </c>
     </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>SG_DT_NONE_PLSR</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>SG+DT</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>PLSR</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>0.9769</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>0.0189</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>0.9317</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>0.0327</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>3.8258</t>
+        </is>
+      </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>0.0253</t>
+        </is>
+      </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>2.9319</t>
+        </is>
+      </c>
+      <c r="L187" t="inlineStr">
+        <is>
+          <t>3.0792</t>
+        </is>
+      </c>
+      <c r="M187" t="inlineStr">
+        <is>
+          <t>3.0797</t>
+        </is>
+      </c>
+      <c r="N187" t="inlineStr">
+        <is>
+          <t>{'method': ['sg', 'dt']}</t>
+        </is>
+      </c>
+      <c r="O187" t="inlineStr">
+        <is>
+          <t>[None]</t>
+        </is>
+      </c>
+      <c r="P187" t="inlineStr">
+        <is>
+          <t>n_comp=30</t>
+        </is>
+      </c>
+      <c r="Q187" t="inlineStr">
+        <is>
+          <t>[0.72 0.72 0.73 0.73 0.72 0.72 0.7  0.7  0.7  0.7  0.64 0.64 0.63 0.63
+ 0.64 0.64 0.62 0.62 0.62 0.62 0.43 0.43 0.46 0.34 0.34 0.31 0.31 0.72
+ 0.72 0.66 0.66 0.62 0.62 0.62 0.62 0.62 0.62 0.58 0.58 0.74 0.74 0.72
+ 0.72 0.72 0.72 0.62 0.62 0.59 0.59 0.53 0.53 0.7  0.7  0.6  0.6  0.61
+ 0.61 0.54 0.54 0.52 0.52 0.51 0.51 0.71 0.71 0.55 0.55 0.63 0.63 0.6
+ 0.6  0.46 0.46 0.73 0.73 0.71 0.71 0.67 0.67 0.59 0.59 0.1  0.1  0.63
+ 0.73 0.46 0.62 0.72 0.61 0.51 0.6  0.46]</t>
+        </is>
+      </c>
+      <c r="R187" t="inlineStr">
+        <is>
+          <t>[[0.78279259]
+ [0.69842338]
+ [0.77171632]
+ [0.74771421]
+ [0.69659771]
+ [0.7344295 ]
+ [0.70092695]
+ [0.62185358]
+ [0.76869509]
+ [0.7475982 ]
+ [0.6417928 ]
+ [0.5765341 ]
+ [0.62247245]
+ [0.65316219]
+ [0.64984981]
+ [0.57909118]
+ [0.69871158]
+ [0.62589845]
+ [0.63547467]
+ [0.67205494]
+ [0.49554376]
+ [0.49504514]
+ [0.40759447]
+ [0.32808319]
+ [0.39423872]
+ [0.35321917]
+ [0.35256582]
+ [0.67830449]
+ [0.71311754]
+ [0.66894115]
+ [0.68642638]
+ [0.61257773]
+ [0.62874943]
+ [0.63482372]
+ [0.60969991]
+ [0.56190536]
+ [0.60667876]
+ [0.61929425]
+ [0.56381747]
+ [0.72912144]
+ [0.74068946]
+ [0.69558299]
+ [0.68020537]
+ [0.69504734]
+ [0.7122183 ]
+ [0.60630474]
+ [0.62015733]
+ [0.63073669]
+ [0.6118014 ]
+ [0.53451807]
+ [0.56434808]
+ [0.69528738]
+ [0.68440327]
+ [0.58516574]
+ [0.56700829]
+ [0.61466187]
+ [0.60969899]
+ [0.58839034]
+ [0.54496067]
+ [0.54500119]
+ [0.48861668]
+ [0.48629985]
+ [0.45308585]
+ [0.67568475]
+ [0.74647821]
+ [0.53153692]
+ [0.5398587 ]
+ [0.57635481]
+ [0.63898493]
+ [0.64982912]
+ [0.63053781]
+ [0.46048744]
+ [0.47305212]
+ [0.72960831]
+ [0.70133272]
+ [0.6787117 ]
+ [0.66291125]
+ [0.68885847]
+ [0.66661132]
+ [0.54457447]
+ [0.55891569]
+ [0.09186618]
+ [0.09854607]
+ [0.62563001]
+ [0.73459577]
+ [0.43090607]
+ [0.6148712 ]
+ [0.71165987]
+ [0.60550618]
+ [0.50330281]
+ [0.61857474]
+ [0.46353455]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>SG_LASSO_PLSR</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>LASSO</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>PLSR</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>0.9655</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>0.0234</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>0.9635</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>0.0239</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>5.2337</t>
+        </is>
+      </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>0.0183</t>
+        </is>
+      </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>1.9707</t>
+        </is>
+      </c>
+      <c r="L188" t="inlineStr">
+        <is>
+          <t>2.0315</t>
+        </is>
+      </c>
+      <c r="M188" t="inlineStr">
+        <is>
+          <t>2.0317</t>
+        </is>
+      </c>
+      <c r="N188" t="inlineStr">
+        <is>
+          <t>{'method': ['sg']}</t>
+        </is>
+      </c>
+      <c r="O188" t="inlineStr">
+        <is>
+          <t>[{'alpha': 0.0005, 'normalize': False}]</t>
+        </is>
+      </c>
+      <c r="P188" t="inlineStr">
+        <is>
+          <t>n_comp=8</t>
+        </is>
+      </c>
+      <c r="Q188" t="inlineStr">
+        <is>
+          <t>[0.72 0.72 0.73 0.73 0.72 0.72 0.7  0.7  0.7  0.7  0.64 0.64 0.63 0.63
+ 0.64 0.64 0.62 0.62 0.62 0.62 0.43 0.43 0.46 0.34 0.34 0.31 0.31 0.72
+ 0.72 0.66 0.66 0.62 0.62 0.62 0.62 0.62 0.62 0.58 0.58 0.74 0.74 0.72
+ 0.72 0.72 0.72 0.62 0.62 0.59 0.59 0.53 0.53 0.7  0.7  0.6  0.6  0.61
+ 0.61 0.54 0.54 0.52 0.52 0.51 0.51 0.71 0.71 0.55 0.55 0.63 0.63 0.6
+ 0.6  0.46 0.46 0.73 0.73 0.71 0.71 0.67 0.67 0.59 0.59 0.1  0.1  0.63
+ 0.73 0.46 0.62 0.72 0.61 0.51 0.6  0.46]</t>
+        </is>
+      </c>
+      <c r="R188" t="inlineStr">
+        <is>
+          <t>[[0.71545736]
+ [0.70898687]
+ [0.74077287]
+ [0.72008441]
+ [0.69949072]
+ [0.73854821]
+ [0.69229279]
+ [0.69514524]
+ [0.71828706]
+ [0.71775247]
+ [0.67128003]
+ [0.62768502]
+ [0.61091465]
+ [0.60189326]
+ [0.65078522]
+ [0.63781563]
+ [0.65129913]
+ [0.64469616]
+ [0.61861766]
+ [0.66211137]
+ [0.48635311]
+ [0.49359267]
+ [0.42095387]
+ [0.37174963]
+ [0.37633605]
+ [0.31121659]
+ [0.31640141]
+ [0.7130768 ]
+ [0.7124537 ]
+ [0.63770392]
+ [0.65825413]
+ [0.62111706]
+ [0.60131418]
+ [0.64177014]
+ [0.64355614]
+ [0.6147127 ]
+ [0.64711607]
+ [0.61590529]
+ [0.57754952]
+ [0.73428934]
+ [0.72722128]
+ [0.7246355 ]
+ [0.71010161]
+ [0.70591437]
+ [0.72931741]
+ [0.60175595]
+ [0.59345173]
+ [0.62880794]
+ [0.59716931]
+ [0.54086073]
+ [0.55357594]
+ [0.69979692]
+ [0.69897663]
+ [0.59889998]
+ [0.58036678]
+ [0.59772809]
+ [0.59780051]
+ [0.59820588]
+ [0.54492776]
+ [0.55266434]
+ [0.51469309]
+ [0.50931836]
+ [0.49578793]
+ [0.69198045]
+ [0.70600617]
+ [0.54379606]
+ [0.55053953]
+ [0.58328099]
+ [0.56962935]
+ [0.63651691]
+ [0.63009846]
+ [0.49714545]
+ [0.48320998]
+ [0.71550712]
+ [0.71636731]
+ [0.70156642]
+ [0.69392275]
+ [0.64454993]
+ [0.68188344]
+ [0.55582664]
+ [0.57515395]
+ [0.09679976]
+ [0.10599744]
+ [0.61423429]
+ [0.7130312 ]
+ [0.40046609]
+ [0.62431629]
+ [0.72436868]
+ [0.59261627]
+ [0.50844822]
+ [0.64221464]
+ [0.49347521]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>SG_LASSO_PLSR</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>LASSO</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>PLSR</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>0.9660</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>0.0232</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>0.9641</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>0.0237</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>5.2809</t>
+        </is>
+      </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>0.0184</t>
+        </is>
+      </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>1.9790</t>
+        </is>
+      </c>
+      <c r="L189" t="inlineStr">
+        <is>
+          <t>2.0333</t>
+        </is>
+      </c>
+      <c r="M189" t="inlineStr">
+        <is>
+          <t>2.0326</t>
+        </is>
+      </c>
+      <c r="N189" t="inlineStr">
+        <is>
+          <t>{'method': ['sg']}</t>
+        </is>
+      </c>
+      <c r="O189" t="inlineStr">
+        <is>
+          <t>[{'alpha': 0.0005, 'normalize': False}]</t>
+        </is>
+      </c>
+      <c r="P189" t="inlineStr">
+        <is>
+          <t>n_comp=11</t>
+        </is>
+      </c>
+      <c r="Q189" t="inlineStr">
+        <is>
+          <t>[0.72 0.72 0.73 0.73 0.72 0.72 0.7  0.7  0.7  0.7  0.64 0.64 0.63 0.63
+ 0.64 0.64 0.62 0.62 0.62 0.62 0.43 0.43 0.46 0.34 0.34 0.31 0.31 0.72
+ 0.72 0.66 0.66 0.62 0.62 0.62 0.62 0.62 0.62 0.58 0.58 0.74 0.74 0.72
+ 0.72 0.72 0.72 0.62 0.62 0.59 0.59 0.53 0.53 0.7  0.7  0.6  0.6  0.61
+ 0.61 0.54 0.54 0.52 0.52 0.51 0.51 0.71 0.71 0.55 0.55 0.63 0.63 0.6
+ 0.6  0.46 0.46 0.73 0.73 0.71 0.71 0.67 0.67 0.59 0.59 0.1  0.1  0.63
+ 0.73 0.46 0.62 0.72 0.61 0.51 0.6  0.46]</t>
+        </is>
+      </c>
+      <c r="R189" t="inlineStr">
+        <is>
+          <t>[[0.72721184]
+ [0.71614959]
+ [0.75266576]
+ [0.72391554]
+ [0.70188385]
+ [0.73093248]
+ [0.68812234]
+ [0.69074794]
+ [0.72783293]
+ [0.71952688]
+ [0.66740802]
+ [0.62576739]
+ [0.60716775]
+ [0.60393128]
+ [0.6526802 ]
+ [0.6335325 ]
+ [0.65931682]
+ [0.63972494]
+ [0.61601348]
+ [0.6542499 ]
+ [0.47369218]
+ [0.4893124 ]
+ [0.41309739]
+ [0.36684198]
+ [0.37484394]
+ [0.31548577]
+ [0.31769943]
+ [0.7082337 ]
+ [0.71239181]
+ [0.63346153]
+ [0.65072281]
+ [0.62075321]
+ [0.60262732]
+ [0.63618555]
+ [0.64392215]
+ [0.61663066]
+ [0.64195517]
+ [0.61281587]
+ [0.579456  ]
+ [0.73634388]
+ [0.72745691]
+ [0.72223101]
+ [0.70815995]
+ [0.70648097]
+ [0.73420815]
+ [0.60105411]
+ [0.59722253]
+ [0.62100803]
+ [0.59317895]
+ [0.54696739]
+ [0.56255577]
+ [0.69701529]
+ [0.70059078]
+ [0.58926203]
+ [0.57780479]
+ [0.60282081]
+ [0.60021997]
+ [0.60348741]
+ [0.53617512]
+ [0.55483658]
+ [0.51709408]
+ [0.50835917]
+ [0.4944148 ]
+ [0.69296301]
+ [0.70979381]
+ [0.54959373]
+ [0.55298178]
+ [0.58516652]
+ [0.56623828]
+ [0.63512301]
+ [0.6298464 ]
+ [0.49580453]
+ [0.48439417]
+ [0.71894192]
+ [0.71583956]
+ [0.70232787]
+ [0.6907815 ]
+ [0.64637198]
+ [0.68852332]
+ [0.55590553]
+ [0.57427208]
+ [0.09449377]
+ [0.10618872]
+ [0.61365285]
+ [0.71800074]
+ [0.40024276]
+ [0.62368713]
+ [0.72220802]
+ [0.5962827 ]
+ [0.50684454]
+ [0.64047157]
+ [0.49094882]]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>